<commit_message>
FastPlot added and run without retrieving new
</commit_message>
<xml_diff>
--- a/Info/Info.xlsx
+++ b/Info/Info.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17895" windowHeight="7560" tabRatio="713" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17895" windowHeight="7560" tabRatio="713" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="setup" sheetId="9" r:id="rId1"/>
@@ -2797,8 +2797,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E39" sqref="E39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2942,8 +2942,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="F60" sqref="F60"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4917,7 +4917,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T153"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="E111" sqref="E111"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Tidied code and fixed png export, pdf to do
</commit_message>
<xml_diff>
--- a/Info/Info.xlsx
+++ b/Info/Info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nms198\Git\ToOLTuBES\Info\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7AEEB54-9657-48F2-AE97-AC77D9BAA7F8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66FD6FD3-8B7A-4F91-8A21-AF1A5E456864}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="713" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="713" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="setup" sheetId="9" r:id="rId1"/>
@@ -21,17 +21,23 @@
     <sheet name="parameters_ave" sheetId="7" r:id="rId6"/>
     <sheet name="colours" sheetId="10" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1539" uniqueCount="610">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1547" uniqueCount="618">
   <si>
     <t>Slim</t>
   </si>
@@ -1879,6 +1885,30 @@
   </si>
   <si>
     <t>diamond</t>
+  </si>
+  <si>
+    <t>refresh_hours</t>
+  </si>
+  <si>
+    <t>png_width</t>
+  </si>
+  <si>
+    <t>png_height</t>
+  </si>
+  <si>
+    <t>pdf_width</t>
+  </si>
+  <si>
+    <t>pdf_height</t>
+  </si>
+  <si>
+    <t>html_fig_width</t>
+  </si>
+  <si>
+    <t>html_height_width</t>
+  </si>
+  <si>
+    <t>last_fig_x</t>
   </si>
 </sst>
 </file>
@@ -2446,10 +2476,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2485,6 +2515,14 @@
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>248</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>610</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -2717,10 +2755,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:O6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2730,9 +2768,15 @@
     <col min="5" max="5" width="19" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="15.88671875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>237</v>
       </c>
@@ -2757,8 +2801,29 @@
       <c r="H1" t="s">
         <v>544</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I1" t="s">
+        <v>611</v>
+      </c>
+      <c r="J1" t="s">
+        <v>612</v>
+      </c>
+      <c r="K1" t="s">
+        <v>613</v>
+      </c>
+      <c r="L1" t="s">
+        <v>614</v>
+      </c>
+      <c r="M1" t="s">
+        <v>615</v>
+      </c>
+      <c r="N1" t="s">
+        <v>616</v>
+      </c>
+      <c r="O1" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -2777,8 +2842,29 @@
       <c r="H2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I2">
+        <v>4000</v>
+      </c>
+      <c r="J2">
+        <v>2250</v>
+      </c>
+      <c r="K2">
+        <v>3507</v>
+      </c>
+      <c r="L2">
+        <v>2481</v>
+      </c>
+      <c r="M2">
+        <v>98</v>
+      </c>
+      <c r="N2">
+        <v>20</v>
+      </c>
+      <c r="O2">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2797,8 +2883,29 @@
       <c r="H3" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I3">
+        <v>4000</v>
+      </c>
+      <c r="J3">
+        <v>2250</v>
+      </c>
+      <c r="K3">
+        <v>3507</v>
+      </c>
+      <c r="L3">
+        <v>2481</v>
+      </c>
+      <c r="M3">
+        <v>98</v>
+      </c>
+      <c r="N3">
+        <v>20</v>
+      </c>
+      <c r="O3">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -2814,8 +2921,29 @@
       <c r="H4" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I4">
+        <v>4000</v>
+      </c>
+      <c r="J4">
+        <v>2250</v>
+      </c>
+      <c r="K4">
+        <v>3507</v>
+      </c>
+      <c r="L4">
+        <v>2481</v>
+      </c>
+      <c r="M4">
+        <v>98</v>
+      </c>
+      <c r="N4">
+        <v>20</v>
+      </c>
+      <c r="O4">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
@@ -2831,8 +2959,29 @@
       <c r="H5" t="s">
         <v>552</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I5">
+        <v>4000</v>
+      </c>
+      <c r="J5">
+        <v>2250</v>
+      </c>
+      <c r="K5">
+        <v>3507</v>
+      </c>
+      <c r="L5">
+        <v>2481</v>
+      </c>
+      <c r="M5">
+        <v>98</v>
+      </c>
+      <c r="N5">
+        <v>20</v>
+      </c>
+      <c r="O5">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
@@ -2854,9 +3003,31 @@
       <c r="H6" t="s">
         <v>545</v>
       </c>
+      <c r="I6">
+        <v>4000</v>
+      </c>
+      <c r="J6">
+        <v>2250</v>
+      </c>
+      <c r="K6">
+        <v>3507</v>
+      </c>
+      <c r="L6">
+        <v>2481</v>
+      </c>
+      <c r="M6">
+        <v>98</v>
+      </c>
+      <c r="N6">
+        <v>20</v>
+      </c>
+      <c r="O6">
+        <v>1.25</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2864,7 +3035,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:Q67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+    <sheetView topLeftCell="A40" workbookViewId="0">
       <selection activeCell="H56" sqref="H56"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Fixed when latest data not available turn off.
</commit_message>
<xml_diff>
--- a/Info/Info.xlsx
+++ b/Info/Info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nms198\Git\ToOLTuBES\Info\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66FD6FD3-8B7A-4F91-8A21-AF1A5E456864}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B376A406-ACE3-48C6-BEAC-1797B674C710}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="713" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="713" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="setup" sheetId="9" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1547" uniqueCount="618">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1549" uniqueCount="620">
   <si>
     <t>Slim</t>
   </si>
@@ -1909,6 +1909,12 @@
   </si>
   <si>
     <t>last_fig_x</t>
+  </si>
+  <si>
+    <t>dpi</t>
+  </si>
+  <si>
+    <t>font_size</t>
   </si>
 </sst>
 </file>
@@ -2755,10 +2761,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:O6"/>
+  <dimension ref="A1:Q6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2776,7 +2782,7 @@
     <col min="14" max="14" width="16.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>237</v>
       </c>
@@ -2822,8 +2828,14 @@
       <c r="O1" t="s">
         <v>617</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P1" t="s">
+        <v>618</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -2843,16 +2855,16 @@
         <v>18</v>
       </c>
       <c r="I2">
-        <v>4000</v>
+        <v>1280</v>
       </c>
       <c r="J2">
-        <v>2250</v>
+        <v>720</v>
       </c>
       <c r="K2">
-        <v>3507</v>
+        <v>794</v>
       </c>
       <c r="L2">
-        <v>2481</v>
+        <v>1123</v>
       </c>
       <c r="M2">
         <v>98</v>
@@ -2863,8 +2875,14 @@
       <c r="O2">
         <v>1.25</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P2">
+        <v>300</v>
+      </c>
+      <c r="Q2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2884,16 +2902,16 @@
         <v>20</v>
       </c>
       <c r="I3">
-        <v>4000</v>
+        <v>1280</v>
       </c>
       <c r="J3">
-        <v>2250</v>
+        <v>720</v>
       </c>
       <c r="K3">
-        <v>3507</v>
+        <v>794</v>
       </c>
       <c r="L3">
-        <v>2481</v>
+        <v>1123</v>
       </c>
       <c r="M3">
         <v>98</v>
@@ -2904,8 +2922,14 @@
       <c r="O3">
         <v>1.25</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P3">
+        <v>300</v>
+      </c>
+      <c r="Q3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -2922,16 +2946,16 @@
         <v>22</v>
       </c>
       <c r="I4">
-        <v>4000</v>
+        <v>1280</v>
       </c>
       <c r="J4">
-        <v>2250</v>
+        <v>720</v>
       </c>
       <c r="K4">
-        <v>3507</v>
+        <v>794</v>
       </c>
       <c r="L4">
-        <v>2481</v>
+        <v>1123</v>
       </c>
       <c r="M4">
         <v>98</v>
@@ -2942,8 +2966,14 @@
       <c r="O4">
         <v>1.25</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P4">
+        <v>300</v>
+      </c>
+      <c r="Q4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
@@ -2960,16 +2990,16 @@
         <v>552</v>
       </c>
       <c r="I5">
-        <v>4000</v>
+        <v>1280</v>
       </c>
       <c r="J5">
-        <v>2250</v>
+        <v>720</v>
       </c>
       <c r="K5">
-        <v>3507</v>
+        <v>794</v>
       </c>
       <c r="L5">
-        <v>2481</v>
+        <v>1123</v>
       </c>
       <c r="M5">
         <v>98</v>
@@ -2980,8 +3010,14 @@
       <c r="O5">
         <v>1.25</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P5">
+        <v>300</v>
+      </c>
+      <c r="Q5">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
@@ -3004,16 +3040,16 @@
         <v>545</v>
       </c>
       <c r="I6">
-        <v>4000</v>
+        <v>1280</v>
       </c>
       <c r="J6">
-        <v>2250</v>
+        <v>720</v>
       </c>
       <c r="K6">
-        <v>3507</v>
+        <v>794</v>
       </c>
       <c r="L6">
-        <v>2481</v>
+        <v>1123</v>
       </c>
       <c r="M6">
         <v>98</v>
@@ -3023,6 +3059,12 @@
       </c>
       <c r="O6">
         <v>1.25</v>
+      </c>
+      <c r="P6">
+        <v>300</v>
+      </c>
+      <c r="Q6">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -3035,8 +3077,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:Q67"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="H56" sqref="H56"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3105,9 +3147,6 @@
       <c r="G2">
         <v>0</v>
       </c>
-      <c r="H2">
-        <v>40</v>
-      </c>
       <c r="I2">
         <v>10</v>
       </c>
@@ -3137,9 +3176,6 @@
       <c r="G3">
         <v>0</v>
       </c>
-      <c r="H3">
-        <v>40</v>
-      </c>
       <c r="I3">
         <v>10</v>
       </c>
@@ -3169,9 +3205,6 @@
       <c r="G4">
         <v>0</v>
       </c>
-      <c r="H4">
-        <v>40</v>
-      </c>
       <c r="I4">
         <v>10</v>
       </c>
@@ -3201,9 +3234,6 @@
       <c r="G5">
         <v>0</v>
       </c>
-      <c r="H5">
-        <v>600</v>
-      </c>
       <c r="I5">
         <v>10</v>
       </c>
@@ -3233,9 +3263,6 @@
       <c r="G6">
         <v>0</v>
       </c>
-      <c r="H6">
-        <v>500</v>
-      </c>
       <c r="I6">
         <v>10</v>
       </c>
@@ -3265,9 +3292,6 @@
       <c r="G7">
         <v>0</v>
       </c>
-      <c r="H7">
-        <v>60</v>
-      </c>
       <c r="I7">
         <v>10</v>
       </c>
@@ -3297,9 +3321,6 @@
       <c r="G8">
         <v>0</v>
       </c>
-      <c r="H8">
-        <v>150</v>
-      </c>
       <c r="I8">
         <v>8</v>
       </c>
@@ -3329,9 +3350,6 @@
       <c r="G9">
         <v>0</v>
       </c>
-      <c r="H9">
-        <v>30</v>
-      </c>
       <c r="I9">
         <v>8</v>
       </c>
@@ -3390,12 +3408,6 @@
       <c r="F11" t="s">
         <v>580</v>
       </c>
-      <c r="G11">
-        <v>-50</v>
-      </c>
-      <c r="H11">
-        <v>50</v>
-      </c>
       <c r="I11">
         <v>10</v>
       </c>
@@ -3457,9 +3469,6 @@
       <c r="G13">
         <v>0</v>
       </c>
-      <c r="H13">
-        <v>2500</v>
-      </c>
       <c r="I13">
         <v>10</v>
       </c>
@@ -3587,9 +3596,6 @@
       </c>
       <c r="G17">
         <v>0</v>
-      </c>
-      <c r="H17">
-        <v>3</v>
       </c>
       <c r="I17">
         <v>10</v>

</xml_diff>